<commit_message>
Update Quiz Dashboard scripts
</commit_message>
<xml_diff>
--- a/FlipApp/testdata/testdata.xlsx
+++ b/FlipApp/testdata/testdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="19">
   <si>
     <t>Key</t>
   </si>
@@ -61,13 +61,16 @@
     <t>iOS</t>
   </si>
   <si>
-    <t>verifyQuizDashBoardClasses</t>
-  </si>
-  <si>
     <t>Quiz Dashboard Classes</t>
   </si>
   <si>
     <t>Class 3-A, Class 3-B, Class 3-C, Class 4-A, Class 4-B, Class 4-C, Class 5-A, Class 5-B, Class 5-C, Class 6-A, Class 6-B, Class 6-C, Class 7-A, Class 7-B, Class 7-C, Class 8-A, Class 8-B, Class 8-C, Class 9-A, Class 9-B, Class 9-C, Class 10-A, Class 10-B, Class 10-C</t>
+  </si>
+  <si>
+    <t>verifyQuizDashboardClasses</t>
+  </si>
+  <si>
+    <t>Class 6-C, Class 7-A</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F17" sqref="F17:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -590,16 +593,16 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
         <v>16</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -607,16 +610,16 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
         <v>16</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -624,16 +627,16 @@
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
       <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
         <v>16</v>
-      </c>
-      <c r="F13" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -641,16 +644,16 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
         <v>16</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -658,16 +661,16 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
       </c>
       <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
         <v>16</v>
-      </c>
-      <c r="F15" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -675,58 +678,67 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
       </c>
       <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
         <v>16</v>
       </c>
-      <c r="F16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
+    </row>
+    <row r="17" spans="2:6">
       <c r="B17" t="s">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
       <c r="B19" t="s">
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added profile refresh test cases
</commit_message>
<xml_diff>
--- a/FlipApp/testdata/testdata.xlsx
+++ b/FlipApp/testdata/testdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="22">
   <si>
     <t>Key</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t>Class 6-C, Class 7-A</t>
+  </si>
+  <si>
+    <t>verifyPrimeClassOnProfileRefresh</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Class 11 Class 12</t>
   </si>
 </sst>
 </file>
@@ -402,15 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -741,6 +750,57 @@
         <v>18</v>
       </c>
     </row>
+    <row r="20" spans="2:6">
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Prime Search test cases
</commit_message>
<xml_diff>
--- a/FlipApp/testdata/testdata.xlsx
+++ b/FlipApp/testdata/testdata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3432BAD0-D035-4FEA-8A7A-D076197CC1B8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AEA10F-9A61-1A45-A143-8E0780D87381}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="31">
   <si>
     <t>Key</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Quiz Dashboard Classes</t>
   </si>
   <si>
-    <t>Class 3-A, Class 3-B, Class 3-C, Class 4-A, Class 4-B, Class 4-C, Class 5-A, Class 5-B, Class 5-C, Class 6-A, Class 6-B, Class 6-C, Class 7-A, Class 7-B, Class 7-C, Class 8-A, Class 8-B, Class 8-C, Class 9-A, Class 9-B, Class 9-C, Class 10-A, Class 10-B, Class 10-C</t>
-  </si>
-  <si>
     <t>verifyQuizDashboardClasses</t>
   </si>
   <si>
@@ -93,6 +90,24 @@
   </si>
   <si>
     <t>Guest</t>
+  </si>
+  <si>
+    <t>Class 3-A, Class 3-B, Class 3-C, Class 4-A, Class 4-B, Class 4-C, Class 5-A, Class 5-B, Class 5-C, Class 6-A, Class 6-B, Class 6-C, Class 7-A, Class 7-B, Class 7-C, Class 8-A, Class 8-B, Class 8-C, Class 9-A, Class 9-B, Class 9-C, Class 10-A, Class 10-B, Class 10-C, Class 11-A, Class 11-B, Class 11-C, Class 12-A, Class 12-B, Class 12-C</t>
+  </si>
+  <si>
+    <t>searchAndViewContentStudent</t>
+  </si>
+  <si>
+    <t>searchAndViewContentSchool</t>
+  </si>
+  <si>
+    <t>Search String</t>
+  </si>
+  <si>
+    <t>Autotrophic Nutrition</t>
+  </si>
+  <si>
+    <t>Making stone tools and the discovery of fire</t>
   </si>
 </sst>
 </file>
@@ -468,20 +483,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -501,7 +516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -518,7 +533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -535,7 +550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>14</v>
       </c>
@@ -552,7 +567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -569,7 +584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -586,7 +601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -603,7 +618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -620,7 +635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -637,7 +652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -654,114 +669,114 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
         <v>20</v>
       </c>
-      <c r="F11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
         <v>20</v>
       </c>
-      <c r="F12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
         <v>20</v>
       </c>
-      <c r="F13" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
         <v>19</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
         <v>24</v>
       </c>
-      <c r="E14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="E16" t="s">
         <v>19</v>
       </c>
-      <c r="D15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
-      </c>
       <c r="F16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
@@ -770,15 +785,15 @@
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
         <v>10</v>
@@ -787,15 +802,15 @@
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -804,15 +819,15 @@
         <v>15</v>
       </c>
       <c r="F19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>17</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -821,15 +836,15 @@
         <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -838,15 +853,15 @@
         <v>15</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -855,15 +870,15 @@
         <v>15</v>
       </c>
       <c r="F22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>17</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
@@ -872,15 +887,15 @@
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
@@ -889,15 +904,15 @@
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
@@ -906,7 +921,313 @@
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" t="s">
+        <v>28</v>
+      </c>
+      <c r="F37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" t="s">
+        <v>28</v>
+      </c>
+      <c r="F41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" t="s">
+        <v>28</v>
+      </c>
+      <c r="F43" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Android test cases for prime and quiz
</commit_message>
<xml_diff>
--- a/FlipApp/testdata/testdata.xlsx
+++ b/FlipApp/testdata/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AEA10F-9A61-1A45-A143-8E0780D87381}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5C7B1A-DC31-1442-B230-9CE24E88F9F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="30">
   <si>
     <t>Key</t>
   </si>
@@ -26,9 +26,6 @@
     <t>Prime Classes</t>
   </si>
   <si>
-    <t>Pre Nursery, Nursery, KG, Class 1, Class 2, Class 3, Class 4, Class 5, Class 6, Class 7, Class 8, Class 9, Class 10, Class 11, Class 12</t>
-  </si>
-  <si>
     <t>Web</t>
   </si>
   <si>
@@ -77,12 +74,6 @@
     <t>Prime Subjects</t>
   </si>
   <si>
-    <t>English,EVS,Hindi,Mathematics</t>
-  </si>
-  <si>
-    <t>English, Hindi, Mathematics, Science, Social Studies</t>
-  </si>
-  <si>
     <t>Student</t>
   </si>
   <si>
@@ -108,6 +99,12 @@
   </si>
   <si>
     <t>Making stone tools and the discovery of fire</t>
+  </si>
+  <si>
+    <t>Pre Nursery, Nursery, KG, Class 1, Class 2, Class 3, Class 4, Class 5, Class 6, Class 7, Class 8, Class 9, Class 10</t>
+  </si>
+  <si>
+    <t>English, Hindi</t>
   </si>
 </sst>
 </file>
@@ -483,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -498,16 +495,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -518,424 +515,424 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F26" t="s">
         <v>29</v>
@@ -943,16 +940,16 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F27" t="s">
         <v>29</v>
@@ -960,16 +957,16 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E28" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F28" t="s">
         <v>29</v>
@@ -977,257 +974,461 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
         <v>14</v>
       </c>
-      <c r="C31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" t="s">
-        <v>28</v>
-      </c>
       <c r="F31" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F32" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F33" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="s">
         <v>14</v>
       </c>
-      <c r="C34" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" t="s">
-        <v>28</v>
-      </c>
       <c r="F34" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F35" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D36" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F36" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
         <v>14</v>
       </c>
-      <c r="C37" t="s">
-        <v>26</v>
-      </c>
-      <c r="D37" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" t="s">
-        <v>28</v>
-      </c>
       <c r="F37" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" t="s">
         <v>26</v>
-      </c>
-      <c r="D38" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" t="s">
-        <v>28</v>
-      </c>
-      <c r="F38" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" t="s">
         <v>26</v>
-      </c>
-      <c r="D39" t="s">
-        <v>22</v>
-      </c>
-      <c r="E39" t="s">
-        <v>28</v>
-      </c>
-      <c r="F39" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" t="s">
         <v>26</v>
-      </c>
-      <c r="D40" t="s">
-        <v>22</v>
-      </c>
-      <c r="E40" t="s">
-        <v>28</v>
-      </c>
-      <c r="F40" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" t="s">
         <v>26</v>
-      </c>
-      <c r="D41" t="s">
-        <v>24</v>
-      </c>
-      <c r="E41" t="s">
-        <v>28</v>
-      </c>
-      <c r="F41" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" t="s">
         <v>26</v>
-      </c>
-      <c r="D42" t="s">
-        <v>24</v>
-      </c>
-      <c r="E42" t="s">
-        <v>28</v>
-      </c>
-      <c r="F42" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C43" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" t="s">
         <v>26</v>
       </c>
-      <c r="D43" t="s">
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
         <v>24</v>
       </c>
-      <c r="E43" t="s">
-        <v>28</v>
-      </c>
-      <c r="F43" t="s">
-        <v>30</v>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" t="s">
+        <v>25</v>
+      </c>
+      <c r="F47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" t="s">
+        <v>25</v>
+      </c>
+      <c r="F51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" t="s">
+        <v>25</v>
+      </c>
+      <c r="F52" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" t="s">
+        <v>21</v>
+      </c>
+      <c r="E53" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" t="s">
+        <v>23</v>
+      </c>
+      <c r="D55" t="s">
+        <v>21</v>
+      </c>
+      <c r="E55" t="s">
+        <v>25</v>
+      </c>
+      <c r="F55" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated existing failed testcases after launchpad release
</commit_message>
<xml_diff>
--- a/FlipApp/testdata/testdata.xlsx
+++ b/FlipApp/testdata/testdata.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADE8557-62A7-414D-B2B4-3E4184A1007F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -82,9 +83,6 @@
     <t>Guest</t>
   </si>
   <si>
-    <t>Class 3-A, Class 3-B, Class 3-C, Class 4-A, Class 4-B, Class 4-C, Class 5-A, Class 5-B, Class 5-C, Class 6-A, Class 6-B, Class 6-C, Class 7-A, Class 7-B, Class 7-C, Class 8-A, Class 8-B, Class 8-C, Class 9-A, Class 9-B, Class 9-C, Class 10-A, Class 10-B, Class 10-C, Class 11-A, Class 11-B, Class 11-C, Class 12-A, Class 12-B, Class 12-C</t>
-  </si>
-  <si>
     <t>searchAndViewContentStudent</t>
   </si>
   <si>
@@ -104,13 +102,16 @@
   </si>
   <si>
     <t>Pre Nursery, Nursery, KG, Class 1, Class 2, Class 3, Class 4, Class 5, Class 6, Class 7, Class 8, Class 9, Class 10, Class 11, Class 12</t>
+  </si>
+  <si>
+    <t>Class 3-A, Class 3-B, Class 3-C, Class 4-A, Class 4-B, Class 4-C, Class 5-A, Class 5-B, Class 5-C, Class 6-A, Class 6-B, Class 6-C, Class 7-A, Class 7-B, Class 7-C, Class 8-A, Class 8-B, Class 8-C, Class 8-D, Class 9-A, Class 9-B, Class 9-C, Class 10-A, Class 10-B, Class 10-C, Class 11-A, Class 11-B, Class 11-C, Class 11-D, Class 12-A, Class 12-B, Class 12-C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,7 +202,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,9 +234,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -267,6 +286,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -442,21 +479,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29:F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="28.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -476,7 +513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -490,10 +527,10 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -507,10 +544,10 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>13</v>
       </c>
@@ -524,10 +561,10 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -541,10 +578,10 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -558,10 +595,10 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -575,10 +612,10 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -592,10 +629,10 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>5</v>
       </c>
@@ -609,10 +646,10 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -626,10 +663,10 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>3</v>
       </c>
@@ -643,10 +680,10 @@
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>5</v>
       </c>
@@ -660,10 +697,10 @@
         <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -677,10 +714,10 @@
         <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>3</v>
       </c>
@@ -694,10 +731,10 @@
         <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>5</v>
       </c>
@@ -711,10 +748,10 @@
         <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -728,10 +765,10 @@
         <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -745,10 +782,10 @@
         <v>18</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>5</v>
       </c>
@@ -762,10 +799,10 @@
         <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>13</v>
       </c>
@@ -779,10 +816,10 @@
         <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>3</v>
       </c>
@@ -796,10 +833,10 @@
         <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>5</v>
       </c>
@@ -813,10 +850,10 @@
         <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>13</v>
       </c>
@@ -830,10 +867,10 @@
         <v>18</v>
       </c>
       <c r="F22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -847,10 +884,10 @@
         <v>18</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>5</v>
       </c>
@@ -864,10 +901,10 @@
         <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>13</v>
       </c>
@@ -881,10 +918,10 @@
         <v>18</v>
       </c>
       <c r="F25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>3</v>
       </c>
@@ -898,10 +935,10 @@
         <v>18</v>
       </c>
       <c r="F26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>3</v>
       </c>
@@ -915,10 +952,10 @@
         <v>18</v>
       </c>
       <c r="F27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>5</v>
       </c>
@@ -932,10 +969,10 @@
         <v>18</v>
       </c>
       <c r="F28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>3</v>
       </c>
@@ -949,10 +986,10 @@
         <v>14</v>
       </c>
       <c r="F29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>5</v>
       </c>
@@ -966,10 +1003,10 @@
         <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>13</v>
       </c>
@@ -983,10 +1020,10 @@
         <v>14</v>
       </c>
       <c r="F31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>3</v>
       </c>
@@ -1000,10 +1037,10 @@
         <v>14</v>
       </c>
       <c r="F32" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>5</v>
       </c>
@@ -1017,10 +1054,10 @@
         <v>14</v>
       </c>
       <c r="F33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>13</v>
       </c>
@@ -1034,10 +1071,10 @@
         <v>14</v>
       </c>
       <c r="F34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>3</v>
       </c>
@@ -1054,7 +1091,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>5</v>
       </c>
@@ -1071,7 +1108,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>13</v>
       </c>
@@ -1088,310 +1125,310 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="2:6">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D38" t="s">
         <v>9</v>
       </c>
       <c r="E38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" t="s">
         <v>25</v>
       </c>
-      <c r="F38" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6">
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
       </c>
       <c r="E39" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" t="s">
         <v>25</v>
       </c>
-      <c r="F39" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6">
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
       </c>
       <c r="E40" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" t="s">
         <v>25</v>
       </c>
-      <c r="F40" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6">
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D41" t="s">
         <v>10</v>
       </c>
       <c r="E41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" t="s">
         <v>25</v>
       </c>
-      <c r="F41" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6">
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D42" t="s">
         <v>10</v>
       </c>
       <c r="E42" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" t="s">
         <v>25</v>
       </c>
-      <c r="F42" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6">
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D43" t="s">
         <v>10</v>
       </c>
       <c r="E43" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" t="s">
         <v>25</v>
       </c>
-      <c r="F43" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6">
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
       </c>
       <c r="E44" t="s">
+        <v>24</v>
+      </c>
+      <c r="F44" t="s">
         <v>25</v>
       </c>
-      <c r="F44" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6">
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
       </c>
       <c r="E45" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" t="s">
         <v>25</v>
       </c>
-      <c r="F45" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6">
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>13</v>
       </c>
       <c r="C46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
       </c>
       <c r="E46" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" t="s">
         <v>25</v>
       </c>
-      <c r="F46" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6">
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D47" t="s">
         <v>20</v>
       </c>
       <c r="E47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F47" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D48" t="s">
         <v>20</v>
       </c>
       <c r="E48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F48" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D49" t="s">
         <v>20</v>
       </c>
       <c r="E49" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F49" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D50" t="s">
         <v>19</v>
       </c>
       <c r="E50" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F50" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D51" t="s">
         <v>19</v>
       </c>
       <c r="E51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F51" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D52" t="s">
         <v>19</v>
       </c>
       <c r="E52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D53" t="s">
         <v>21</v>
       </c>
       <c r="E53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F53" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D54" t="s">
         <v>21</v>
       </c>
       <c r="E54" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F54" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D55" t="s">
         <v>21</v>
       </c>
       <c r="E55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F55" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated existing test cases for prime module
</commit_message>
<xml_diff>
--- a/FlipApp/testdata/testdata.xlsx
+++ b/FlipApp/testdata/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADE8557-62A7-414D-B2B4-3E4184A1007F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC96A09B-9C75-E341-BCBD-C1E97E26A129}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Teacher</t>
   </si>
   <si>
-    <t>verifyPrimeClasses</t>
-  </si>
-  <si>
     <t>iOS</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>Class 5-C, Class 6-A</t>
   </si>
   <si>
-    <t>verifyPrimeSubjects</t>
-  </si>
-  <si>
     <t>Prime Subjects</t>
   </si>
   <si>
@@ -83,12 +77,6 @@
     <t>Guest</t>
   </si>
   <si>
-    <t>searchAndViewContentStudent</t>
-  </si>
-  <si>
-    <t>searchAndViewContentSchool</t>
-  </si>
-  <si>
     <t>Search String</t>
   </si>
   <si>
@@ -105,6 +93,18 @@
   </si>
   <si>
     <t>Class 3-A, Class 3-B, Class 3-C, Class 4-A, Class 4-B, Class 4-C, Class 5-A, Class 5-B, Class 5-C, Class 6-A, Class 6-B, Class 6-C, Class 7-A, Class 7-B, Class 7-C, Class 8-A, Class 8-B, Class 8-C, Class 8-D, Class 9-A, Class 9-B, Class 9-C, Class 10-A, Class 10-B, Class 10-C, Class 11-A, Class 11-B, Class 11-C, Class 11-D, Class 12-A, Class 12-B, Class 12-C</t>
+  </si>
+  <si>
+    <t>verifyPrimeClasses_Old</t>
+  </si>
+  <si>
+    <t>verifyPrimeSubjects_Old</t>
+  </si>
+  <si>
+    <t>searchAndViewContentSchool_Old</t>
+  </si>
+  <si>
+    <t>searchAndViewContentStudent_Old</t>
   </si>
 </sst>
 </file>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29:F34"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -518,7 +518,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -527,7 +527,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -535,7 +535,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -544,15 +544,15 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -561,7 +561,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -569,7 +569,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -578,7 +578,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -586,7 +586,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -595,15 +595,15 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -612,7 +612,7 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -620,7 +620,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -629,7 +629,7 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -637,7 +637,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -646,15 +646,15 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -663,7 +663,7 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -671,16 +671,16 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -688,33 +688,33 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -722,16 +722,16 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -739,33 +739,33 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -773,16 +773,16 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
@@ -790,33 +790,33 @@
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
@@ -824,16 +824,16 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
@@ -841,33 +841,33 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
@@ -875,16 +875,16 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
         <v>17</v>
       </c>
-      <c r="D23" t="s">
-        <v>19</v>
-      </c>
       <c r="E23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
@@ -892,33 +892,33 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" t="s">
         <v>17</v>
       </c>
-      <c r="D24" t="s">
-        <v>19</v>
-      </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
         <v>17</v>
       </c>
-      <c r="D25" t="s">
-        <v>19</v>
-      </c>
       <c r="E25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F25" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
@@ -926,16 +926,16 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
@@ -943,16 +943,16 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F27" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
@@ -960,16 +960,16 @@
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E28" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F28" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
@@ -977,16 +977,16 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F29" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
@@ -994,33 +994,33 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F30" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
       </c>
       <c r="E31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F31" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
@@ -1028,16 +1028,16 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F32" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
@@ -1045,33 +1045,33 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F33" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F34" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
@@ -1079,16 +1079,16 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
@@ -1096,33 +1096,33 @@
         <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
@@ -1130,16 +1130,16 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D38" t="s">
         <v>9</v>
       </c>
       <c r="E38" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F38" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
@@ -1147,33 +1147,33 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
       </c>
       <c r="E39" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F39" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D40" t="s">
         <v>9</v>
       </c>
       <c r="E40" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F40" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
@@ -1181,16 +1181,16 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D41" t="s">
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F41" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
@@ -1198,33 +1198,33 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D42" t="s">
         <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F42" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D43" t="s">
         <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F43" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.2">
@@ -1232,16 +1232,16 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
       </c>
       <c r="E44" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F44" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.2">
@@ -1249,33 +1249,33 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
       </c>
       <c r="E45" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F45" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F46" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.2">
@@ -1283,16 +1283,16 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" t="s">
         <v>22</v>
-      </c>
-      <c r="D47" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47" t="s">
-        <v>24</v>
-      </c>
-      <c r="F47" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.2">
@@ -1300,33 +1300,33 @@
         <v>5</v>
       </c>
       <c r="C48" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" t="s">
         <v>22</v>
-      </c>
-      <c r="D48" t="s">
-        <v>20</v>
-      </c>
-      <c r="E48" t="s">
-        <v>24</v>
-      </c>
-      <c r="F48" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C49" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" t="s">
         <v>22</v>
-      </c>
-      <c r="D49" t="s">
-        <v>20</v>
-      </c>
-      <c r="E49" t="s">
-        <v>24</v>
-      </c>
-      <c r="F49" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.2">
@@ -1334,16 +1334,16 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" t="s">
         <v>22</v>
-      </c>
-      <c r="D50" t="s">
-        <v>19</v>
-      </c>
-      <c r="E50" t="s">
-        <v>24</v>
-      </c>
-      <c r="F50" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.2">
@@ -1351,33 +1351,33 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D51" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" t="s">
         <v>22</v>
-      </c>
-      <c r="D51" t="s">
-        <v>19</v>
-      </c>
-      <c r="E51" t="s">
-        <v>24</v>
-      </c>
-      <c r="F51" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" t="s">
         <v>22</v>
-      </c>
-      <c r="D52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E52" t="s">
-        <v>24</v>
-      </c>
-      <c r="F52" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.2">
@@ -1385,16 +1385,16 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" t="s">
         <v>22</v>
-      </c>
-      <c r="D53" t="s">
-        <v>21</v>
-      </c>
-      <c r="E53" t="s">
-        <v>24</v>
-      </c>
-      <c r="F53" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.2">
@@ -1402,33 +1402,33 @@
         <v>5</v>
       </c>
       <c r="C54" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" t="s">
         <v>22</v>
-      </c>
-      <c r="D54" t="s">
-        <v>21</v>
-      </c>
-      <c r="E54" t="s">
-        <v>24</v>
-      </c>
-      <c r="F54" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D55" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" t="s">
         <v>22</v>
-      </c>
-      <c r="D55" t="s">
-        <v>21</v>
-      </c>
-      <c r="E55" t="s">
-        <v>24</v>
-      </c>
-      <c r="F55" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated home test cases
</commit_message>
<xml_diff>
--- a/FlipApp/testdata/testdata.xlsx
+++ b/FlipApp/testdata/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC96A09B-9C75-E341-BCBD-C1E97E26A129}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8DF471-5958-BA43-B1B6-3CF6846FDA98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="31">
   <si>
     <t>Key</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>searchAndViewContentStudent_Old</t>
+  </si>
+  <si>
+    <t>Pre Nursery, Nursery, KG, Class 1, Class 2, Class 3, Class 4, Class 5, Class 6, Class 7, Class 8, Class 9, Class 10</t>
   </si>
 </sst>
 </file>
@@ -482,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -544,7 +547,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -595,7 +598,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -646,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated failed scripts for web
</commit_message>
<xml_diff>
--- a/FlipApp/testdata/testdata.xlsx
+++ b/FlipApp/testdata/testdata.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8DF471-5958-BA43-B1B6-3CF6846FDA98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4625040F-5200-4D44-A651-3ED9741A8210}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="33">
   <si>
     <t>Key</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Pre Nursery, Nursery, KG, Class 1, Class 2, Class 3, Class 4, Class 5, Class 6, Class 7, Class 8, Class 9, Class 10</t>
+  </si>
+  <si>
+    <t>Class 5, Class 6, Class 7</t>
+  </si>
+  <si>
+    <t>verifyPrimeClasses_Parent</t>
   </si>
 </sst>
 </file>
@@ -483,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -674,16 +680,16 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -691,16 +697,16 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -708,16 +714,16 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -728,7 +734,7 @@
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
@@ -745,7 +751,7 @@
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" t="s">
         <v>16</v>
@@ -762,7 +768,7 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" t="s">
         <v>16</v>
@@ -779,7 +785,7 @@
         <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
         <v>16</v>
@@ -796,7 +802,7 @@
         <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
         <v>16</v>
@@ -813,7 +819,7 @@
         <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
         <v>16</v>
@@ -830,7 +836,7 @@
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
         <v>16</v>
@@ -847,7 +853,7 @@
         <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
@@ -864,7 +870,7 @@
         <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
         <v>16</v>
@@ -881,7 +887,7 @@
         <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E23" t="s">
         <v>16</v>
@@ -898,7 +904,7 @@
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E24" t="s">
         <v>16</v>
@@ -915,7 +921,7 @@
         <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E25" t="s">
         <v>16</v>
@@ -932,7 +938,7 @@
         <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
         <v>16</v>
@@ -943,13 +949,13 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
         <v>27</v>
       </c>
       <c r="D27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s">
         <v>16</v>
@@ -960,13 +966,13 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E28" t="s">
         <v>16</v>
@@ -980,50 +986,50 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E30" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E31" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
@@ -1034,7 +1040,7 @@
         <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E32" t="s">
         <v>13</v>
@@ -1051,7 +1057,7 @@
         <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E33" t="s">
         <v>13</v>
@@ -1068,7 +1074,7 @@
         <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E34" t="s">
         <v>13</v>
@@ -1085,13 +1091,13 @@
         <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
@@ -1102,13 +1108,13 @@
         <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E36" t="s">
         <v>13</v>
       </c>
       <c r="F36" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
@@ -1119,13 +1125,13 @@
         <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E37" t="s">
         <v>13</v>
       </c>
       <c r="F37" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
@@ -1133,16 +1139,16 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E38" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F38" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
@@ -1150,16 +1156,16 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E39" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F39" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
@@ -1167,16 +1173,16 @@
         <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E40" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F40" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
@@ -1187,7 +1193,7 @@
         <v>28</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E41" t="s">
         <v>20</v>
@@ -1204,7 +1210,7 @@
         <v>28</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E42" t="s">
         <v>20</v>
@@ -1221,7 +1227,7 @@
         <v>28</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E43" t="s">
         <v>20</v>
@@ -1238,7 +1244,7 @@
         <v>28</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E44" t="s">
         <v>20</v>
@@ -1255,7 +1261,7 @@
         <v>28</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E45" t="s">
         <v>20</v>
@@ -1272,7 +1278,7 @@
         <v>28</v>
       </c>
       <c r="D46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E46" t="s">
         <v>20</v>
@@ -1286,16 +1292,16 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D47" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E47" t="s">
         <v>20</v>
       </c>
       <c r="F47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.2">
@@ -1303,16 +1309,16 @@
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D48" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E48" t="s">
         <v>20</v>
       </c>
       <c r="F48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.2">
@@ -1320,16 +1326,16 @@
         <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D49" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E49" t="s">
         <v>20</v>
       </c>
       <c r="F49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.2">
@@ -1340,7 +1346,7 @@
         <v>29</v>
       </c>
       <c r="D50" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E50" t="s">
         <v>20</v>
@@ -1357,7 +1363,7 @@
         <v>29</v>
       </c>
       <c r="D51" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E51" t="s">
         <v>20</v>
@@ -1374,7 +1380,7 @@
         <v>29</v>
       </c>
       <c r="D52" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E52" t="s">
         <v>20</v>
@@ -1391,7 +1397,7 @@
         <v>29</v>
       </c>
       <c r="D53" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E53" t="s">
         <v>20</v>
@@ -1408,7 +1414,7 @@
         <v>29</v>
       </c>
       <c r="D54" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E54" t="s">
         <v>20</v>
@@ -1425,12 +1431,63 @@
         <v>29</v>
       </c>
       <c r="D55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>29</v>
+      </c>
+      <c r="D56" t="s">
         <v>19</v>
       </c>
-      <c r="E55" t="s">
-        <v>20</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="E56" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" t="s">
+        <v>20</v>
+      </c>
+      <c r="F57" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" t="s">
+        <v>29</v>
+      </c>
+      <c r="D58" t="s">
+        <v>19</v>
+      </c>
+      <c r="E58" t="s">
+        <v>20</v>
+      </c>
+      <c r="F58" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added doubt forum test data
</commit_message>
<xml_diff>
--- a/FlipApp/testdata/testdata.xlsx
+++ b/FlipApp/testdata/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABC9947-1143-564A-B6C7-DB5EE18AC6E4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CF3866-3ED7-6744-A856-F10D260F9396}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="36">
   <si>
     <t>Key</t>
   </si>
@@ -506,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1527,13 +1527,13 @@
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
         <v>34</v>
       </c>
       <c r="D60" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E60" t="s">
         <v>35</v>
@@ -1550,12 +1550,29 @@
         <v>34</v>
       </c>
       <c r="D61" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" t="s">
+        <v>35</v>
+      </c>
+      <c r="F61" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" t="s">
         <v>19</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F62" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated failed guest login testcases
</commit_message>
<xml_diff>
--- a/FlipApp/testdata/testdata.xlsx
+++ b/FlipApp/testdata/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CF3866-3ED7-6744-A856-F10D260F9396}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8777AC44-D4A5-2B41-A6A0-4B52CBBBF0CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="38">
   <si>
     <t>Key</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>DoubtForum Tabs</t>
+  </si>
+  <si>
+    <t>Doubts, My Doubts, Posts For Me</t>
+  </si>
+  <si>
+    <t>Doubts, My Doubts</t>
   </si>
 </sst>
 </file>
@@ -509,7 +515,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1522,7 +1528,7 @@
         <v>35</v>
       </c>
       <c r="F59" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.2">
@@ -1556,7 +1562,7 @@
         <v>35</v>
       </c>
       <c r="F61" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.2">
@@ -1573,7 +1579,7 @@
         <v>35</v>
       </c>
       <c r="F62" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated quiz dashboard test cases
</commit_message>
<xml_diff>
--- a/FlipApp/testdata/testdata.xlsx
+++ b/FlipApp/testdata/testdata.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8777AC44-D4A5-2B41-A6A0-4B52CBBBF0CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AC9C00-1130-1A4C-B21B-568C57B39500}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="production" sheetId="1" r:id="rId1"/>
+    <sheet name="staging" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="39">
   <si>
     <t>Key</t>
   </si>
@@ -129,6 +130,9 @@
   </si>
   <si>
     <t>Doubts, My Doubts</t>
+  </si>
+  <si>
+    <t>Class 3-A, Class 3-A, Class 3-A, Class 3-A, Class 3-B, Class 3-B, Class 3-B, Class 3-B, Class 3-C, Class 3-C, Class 3-C, Class 4-A, Class 4-A, Class 4-A, Class 4-A, Class 4-B, Class 4-B, Class 4-B, Class 4-B, Class 4-C, Class 4-C, Class 4-C, Class 4-C, Class 5-A, Class 5-A, Class 5-A, Class 5-A, Class 5-B, Class 5-B, Class 5-B, Class 5-B, Class 5-C, Class 5-C, Class 5-C, Class 5-C, Class 6-A, Class 6-A, Class 6-A, Class 6-A, Class 6-B, Class 6-B, Class 6-B, Class 6-B, Class 6-C, Class 6-C, Class 6-C, Class 6-C, Class 7-A, Class 7-A, Class 7-A, Class 7-A, Class 7-B, Class 7-B, Class 7-B, Class 7-B, Class 7-C, Class 7-C, Class 7-C, Class 7-C, Class 8-A, Class 8-A, Class 8-A, Class 8-A, Class 8-B, Class 8-B, Class 8-B, Class 8-B, Class 8-C, Class 8-C, Class 8-C, Class 8-C, Class 9-A, Class 9-A, Class 9-A, Class 9-A, Class 9-B, Class 9-B, Class 9-B, Class 9-B, Class 9-C, Class 9-C, Class 9-C, Class 9-C, Class 10-A, Class 10-A, Class 10-B, Class 10-B, Class 10-C, Class 10-C, Class 11-A, Class 11-A, Class 11-A, Class 11-A, Class 11-B, Class 11-B, Class 11-B, Class 11-B, Class 11-C, Class 11-C, Class 11-C, Class 11-C, Class 12-A, Class 12-A, Class 12-A, Class 12-A, Class 12-B, Class 12-B, Class 12-B, Class 12-B, Class 12-C, Class 12-C, Class 12-C</t>
   </si>
 </sst>
 </file>
@@ -514,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1585,4 +1589,1076 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A005F3E-F802-CF40-84CE-148E37BF6DB4}">
+  <dimension ref="A1:F62"/>
+  <sheetViews>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D51" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" t="s">
+        <v>29</v>
+      </c>
+      <c r="D55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>29</v>
+      </c>
+      <c r="D56" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" t="s">
+        <v>20</v>
+      </c>
+      <c r="F57" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" t="s">
+        <v>29</v>
+      </c>
+      <c r="D58" t="s">
+        <v>19</v>
+      </c>
+      <c r="E58" t="s">
+        <v>20</v>
+      </c>
+      <c r="F58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>34</v>
+      </c>
+      <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
+        <v>35</v>
+      </c>
+      <c r="F59" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s">
+        <v>34</v>
+      </c>
+      <c r="D60" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" t="s">
+        <v>35</v>
+      </c>
+      <c r="F60" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D61" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" t="s">
+        <v>35</v>
+      </c>
+      <c r="F61" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F62" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed parent related failed scripts
</commit_message>
<xml_diff>
--- a/FlipApp/testdata/testdata.xlsx
+++ b/FlipApp/testdata/testdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DC857C-8B65-054F-BC9D-82BE3D97DF8E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35DA907-6CE8-294B-B82C-731AF2B1BAE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="13180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="40">
   <si>
     <t>Key</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>verifyDoubtForumTabs</t>
+  </si>
+  <si>
+    <t>Class 4-B, Class 4-C, Class 5-A, Class 5-B, Class 5-C, Class 6-A</t>
   </si>
 </sst>
 </file>
@@ -518,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59:F62"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1175,7 +1178,7 @@
         <v>13</v>
       </c>
       <c r="F38" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
@@ -1192,7 +1195,7 @@
         <v>13</v>
       </c>
       <c r="F39" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
@@ -1209,7 +1212,7 @@
         <v>13</v>
       </c>
       <c r="F40" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
@@ -1595,8 +1598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A005F3E-F802-CF40-84CE-148E37BF6DB4}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59:F62"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>